<commit_message>
New project V3.1.0 Nuevo metodo para ejecutar un caso con varios datos
</commit_message>
<xml_diff>
--- a/data/Navigate Data.xlsx
+++ b/data/Navigate Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MiguelTorres\Documents\SELENIUM PROJECTS\Gradle-Tutorial-IntelliJIDEA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2819C2A3-D92D-49E7-AA81-DE165BB25631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2292478B-A55B-4F73-A61B-E9F4BC47BEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B1DF2AA4-C70B-484D-9A4D-659B17A6743A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1DF2AA4-C70B-484D-9A4D-659B17A6743A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>chrome</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>firefox</t>
   </si>
   <si>
     <t>Test Case Name1</t>
@@ -435,7 +432,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +444,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -458,7 +455,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -469,7 +466,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -480,10 +477,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -491,7 +488,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -502,7 +499,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
New project V3.1.3 Se agrego un metodo public para cerrar los navegadores una vez se ejecuta la prueba en el loop
</commit_message>
<xml_diff>
--- a/data/Navigate Data.xlsx
+++ b/data/Navigate Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MiguelTorres\Documents\SELENIUM PROJECTS\Gradle-Tutorial-IntelliJIDEA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2292478B-A55B-4F73-A61B-E9F4BC47BEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11B2E08-984D-450B-9763-2FB6D1CD56AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1DF2AA4-C70B-484D-9A4D-659B17A6743A}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B1DF2AA4-C70B-484D-9A4D-659B17A6743A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="P7" sqref="P6:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>